<commit_message>
Updated a few tables to make it closer to our DB design
</commit_message>
<xml_diff>
--- a/VideoGameData.xlsx
+++ b/VideoGameData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samga\Google Drive\Weber\CS 3550 - Adv Database Programming\GroupAssignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slamr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE62EA5-463C-4F14-A475-7AB97EE0FD54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210CC5C4-5848-4D49-ABC8-C2663F98F2C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{2D0874AA-25E2-4ECD-8491-5041E3F75BDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{2D0874AA-25E2-4ECD-8491-5041E3F75BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="56">
-  <si>
-    <t>Consoles</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t>ConsoleID</t>
   </si>
@@ -48,21 +45,9 @@
     <t>GameTitle</t>
   </si>
   <si>
-    <t>ConsoleId</t>
-  </si>
-  <si>
     <t>Rating</t>
   </si>
   <si>
-    <t>NumberOfPlayers</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Purchases</t>
-  </si>
-  <si>
     <t>GameID</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>Mario Party</t>
   </si>
   <si>
-    <t>PurchaseID</t>
-  </si>
-  <si>
     <t>Gamecube</t>
   </si>
   <si>
@@ -193,6 +175,105 @@
   </si>
   <si>
     <t>Kmart</t>
+  </si>
+  <si>
+    <t>Sega</t>
+  </si>
+  <si>
+    <t>Genisis</t>
+  </si>
+  <si>
+    <t>Game Gear</t>
+  </si>
+  <si>
+    <t>Atari</t>
+  </si>
+  <si>
+    <t>Magnavox</t>
+  </si>
+  <si>
+    <t>Odyssey</t>
+  </si>
+  <si>
+    <t>ConsoleRefID</t>
+  </si>
+  <si>
+    <t>Console_Ref</t>
+  </si>
+  <si>
+    <t>GameRefID</t>
+  </si>
+  <si>
+    <t>PlayerNumber</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>IsOnline</t>
+  </si>
+  <si>
+    <t>Asteroids</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Dig Dug</t>
+  </si>
+  <si>
+    <t>Shootout!</t>
+  </si>
+  <si>
+    <t>Analogic</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>ESRB</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mature</t>
+  </si>
+  <si>
+    <t>Everyone 10 and up</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>Early Childhood</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Teen</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>Adults Only</t>
+  </si>
+  <si>
+    <t>E10+</t>
+  </si>
+  <si>
+    <t>GamePurchases</t>
+  </si>
+  <si>
+    <t>ConsolePurchases</t>
+  </si>
+  <si>
+    <t>Radio Shack</t>
   </si>
 </sst>
 </file>
@@ -231,19 +312,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="d\-mmm\-yy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -257,10 +350,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A137BEC-C347-4F14-B641-F2CCDDA82B45}" name="Table2" displayName="Table2" ref="A2:D9" totalsRowShown="0">
-  <autoFilter ref="A2:D9" xr:uid="{331A8DFD-96B2-4B0B-91F6-8A4073B1E2CD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8A137BEC-C347-4F14-B641-F2CCDDA82B45}" name="Table2" displayName="Table2" ref="A2:D17" totalsRowShown="0">
+  <autoFilter ref="A2:D17" xr:uid="{331A8DFD-96B2-4B0B-91F6-8A4073B1E2CD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{22CBEA43-4A02-4DA2-B222-D62A50EABCB6}" name="ConsoleID"/>
+    <tableColumn id="1" xr3:uid="{22CBEA43-4A02-4DA2-B222-D62A50EABCB6}" name="ConsoleRefID"/>
     <tableColumn id="2" xr3:uid="{D82B2795-3407-4D29-BBAD-F193CC80DB0B}" name="ConsoleBrand"/>
     <tableColumn id="3" xr3:uid="{B4F92EF5-50B0-4279-845D-405C158BDE33}" name="ConsoleModel"/>
     <tableColumn id="4" xr3:uid="{2B2FCA88-F82C-4FD1-9499-8EF21D9B7B26}" name="SubModel"/>
@@ -270,30 +363,66 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3933C6F8-BA7F-478C-9D02-D889D2DB34E8}" name="Table3" displayName="Table3" ref="G2:L13" totalsRowShown="0">
-  <autoFilter ref="G2:L13" xr:uid="{6044BB5E-06CD-4700-BC76-9E7739202459}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3933C6F8-BA7F-478C-9D02-D889D2DB34E8}" name="Table3" displayName="Table3" ref="G2:J19" totalsRowShown="0">
+  <autoFilter ref="G2:J19" xr:uid="{6044BB5E-06CD-4700-BC76-9E7739202459}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7B6C5D40-8482-4C8F-9BCF-E5A4BCCFC340}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{31940DA7-9FC6-497F-AE61-DF6930CD8FA1}" name="GameTitle"/>
-    <tableColumn id="3" xr3:uid="{DC653776-0A40-4E35-8B79-F3BE0D6F3626}" name="ConsoleId"/>
-    <tableColumn id="4" xr3:uid="{6B6E4433-966B-440D-A38E-7431E6F08017}" name="Rating"/>
-    <tableColumn id="5" xr3:uid="{139DA28B-3C16-44DF-A4BF-14F99B46AE1D}" name="NumberOfPlayers"/>
-    <tableColumn id="6" xr3:uid="{07FADA07-DA1C-4A40-B4E5-7F1871E445BE}" name="Category"/>
+    <tableColumn id="3" xr3:uid="{DC653776-0A40-4E35-8B79-F3BE0D6F3626}" name="Rating"/>
+    <tableColumn id="4" xr3:uid="{6B6E4433-966B-440D-A38E-7431E6F08017}" name="Genre"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:S14" totalsRowShown="0">
-  <autoFilter ref="N2:S14" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
-  <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{95B73333-9D34-4462-BA3A-3674305CC717}" name="PurchaseID"/>
-    <tableColumn id="1" xr3:uid="{8A7CE75F-A322-4402-8FAD-DB517448B052}" name="GameID"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:R14" totalsRowShown="0">
+  <autoFilter ref="N2:R14" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
+  <tableColumns count="5">
+    <tableColumn id="6" xr3:uid="{95B73333-9D34-4462-BA3A-3674305CC717}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{8F2DEC62-0DD3-4939-A7EC-C652AA40CE7C}" name="ConsoleID"/>
     <tableColumn id="3" xr3:uid="{33C14155-BD19-4A59-873F-3B2D4888804F}" name="PurchaseDate"/>
     <tableColumn id="4" xr3:uid="{DDE18AE7-6020-4DB6-B0A7-165C024D9FD3}" name="PurchasePrice"/>
     <tableColumn id="5" xr3:uid="{E0FA8D72-118E-45CB-9428-D2918290DFC1}" name="PurchaseStore"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD363EAC-79ED-4282-BD50-7AECCC8A3080}" name="Table32" displayName="Table32" ref="G24:L42" totalsRowShown="0">
+  <autoFilter ref="G24:L42" xr:uid="{4FBBA3C7-79B4-49CF-ADF9-9C6A8B34225D}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E9010659-292A-491D-A304-998FDA0DFCB9}" name="GameID"/>
+    <tableColumn id="2" xr3:uid="{6B0C8F03-63B7-472D-9B7F-164D8C9739E3}" name="GameRefID"/>
+    <tableColumn id="3" xr3:uid="{61B1A261-4EFC-4008-8B8A-C1C31635D845}" name="ConsoleRefID"/>
+    <tableColumn id="5" xr3:uid="{20D426BE-24EE-40E6-ACC3-3997B9CF1250}" name="PlayerNumber"/>
+    <tableColumn id="6" xr3:uid="{B7203B2C-351E-4D7A-B6C2-3DA4D9305B40}" name="Genre"/>
+    <tableColumn id="4" xr3:uid="{6A9AADC8-8893-4128-8A16-044C3C699010}" name="IsOnline"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5BAE8704-410B-4CAD-B58D-62840EB58D3E}" name="Table326" displayName="Table326" ref="N24:O30" totalsRowShown="0">
+  <autoFilter ref="N24:O30" xr:uid="{E984971F-04B5-411A-B867-E2CA8F0E8375}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{160200E6-5C9A-473B-9635-E9DD681565D6}" name="Rating"/>
+    <tableColumn id="2" xr3:uid="{E21DF097-6EF2-428B-B987-AE9AAF338A46}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D095B64D-2FEB-43CD-A495-6839B1A27E11}" name="Table47" displayName="Table47" ref="A23:D36" totalsRowShown="0">
+  <autoFilter ref="A23:D36" xr:uid="{4788E827-78B0-45DE-AAD1-156376861332}"/>
+  <tableColumns count="4">
+    <tableColumn id="6" xr3:uid="{48246F78-C9C5-42FB-8467-298E310F3747}" name="ConsoleID"/>
+    <tableColumn id="2" xr3:uid="{A3E5494F-2CEB-4C8D-A205-95E6C2666284}" name="PurchaseDate" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{07825330-3684-4A8C-8F99-B7BE0C4BF5EB}" name="PurchasePrice" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{CDD07CE3-7841-492D-92A3-A490D71697D6}" name="PurchaseStore"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,156 +725,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732A0381-8E3F-4A64-ABD3-42AC0D0E900F}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" customWidth="1"/>
-    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="11" max="11" width="17.77734375" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" t="s">
+      <c r="R2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
         <v>2</v>
       </c>
+      <c r="P3" s="2">
+        <v>39391</v>
+      </c>
       <c r="Q3" s="3">
-        <v>39391</v>
-      </c>
-      <c r="R3" s="4">
         <v>50</v>
       </c>
-      <c r="S3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>360</v>
@@ -754,45 +868,39 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
         <v>5</v>
       </c>
+      <c r="P4" s="2">
+        <v>37564</v>
+      </c>
       <c r="Q4" s="3">
-        <v>37564</v>
-      </c>
-      <c r="R4" s="4">
         <v>50</v>
       </c>
-      <c r="S4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -801,133 +909,115 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="N5">
         <v>3</v>
       </c>
       <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
         <v>4</v>
       </c>
+      <c r="P5" s="2">
+        <v>36147</v>
+      </c>
       <c r="Q5" s="3">
-        <v>36147</v>
-      </c>
-      <c r="R5" s="4">
         <v>40</v>
       </c>
-      <c r="S5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N6">
         <v>4</v>
       </c>
       <c r="O6">
-        <v>4</v>
-      </c>
-      <c r="P6">
         <v>1</v>
       </c>
+      <c r="P6" s="2">
+        <v>42797</v>
+      </c>
       <c r="Q6" s="3">
-        <v>42797</v>
-      </c>
-      <c r="R6" s="4">
         <v>60</v>
       </c>
-      <c r="S6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N7">
         <v>5</v>
       </c>
       <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="P7">
         <v>4</v>
       </c>
+      <c r="P7" s="2">
+        <v>36120</v>
+      </c>
       <c r="Q7" s="3">
-        <v>36120</v>
-      </c>
-      <c r="R7" s="4">
         <v>50</v>
       </c>
-      <c r="S7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -936,252 +1026,887 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
       </c>
       <c r="J8" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" t="s">
-        <v>40</v>
-      </c>
       <c r="N8">
         <v>6</v>
       </c>
       <c r="O8">
-        <v>6</v>
-      </c>
-      <c r="P8">
         <v>5</v>
       </c>
+      <c r="P8" s="2">
+        <v>31303</v>
+      </c>
       <c r="Q8" s="3">
-        <v>31303</v>
-      </c>
-      <c r="R8" s="4">
         <v>20</v>
       </c>
-      <c r="S8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G9">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N9">
         <v>7</v>
       </c>
       <c r="O9">
-        <v>7</v>
-      </c>
-      <c r="P9">
         <v>2</v>
       </c>
+      <c r="P9" s="2">
+        <v>40858</v>
+      </c>
       <c r="Q9" s="3">
-        <v>40858</v>
-      </c>
-      <c r="R9" s="4">
         <v>60</v>
       </c>
-      <c r="S9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
       <c r="G10">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N10">
         <v>8</v>
       </c>
       <c r="O10">
-        <v>8</v>
-      </c>
-      <c r="P10">
         <v>4</v>
       </c>
+      <c r="P10" s="2">
+        <v>35471</v>
+      </c>
       <c r="Q10" s="3">
-        <v>35471</v>
-      </c>
-      <c r="R10" s="4">
         <v>40</v>
       </c>
-      <c r="S10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
       <c r="G11">
         <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="N11">
         <v>9</v>
       </c>
       <c r="O11">
-        <v>9</v>
-      </c>
-      <c r="P11">
         <v>6</v>
       </c>
+      <c r="P11" s="2">
+        <v>37516</v>
+      </c>
       <c r="Q11" s="3">
-        <v>37516</v>
-      </c>
-      <c r="R11" s="4">
         <v>60</v>
       </c>
-      <c r="S11" t="s">
+      <c r="R11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
       <c r="G12">
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N12">
         <v>10</v>
       </c>
       <c r="O12">
-        <v>10</v>
-      </c>
-      <c r="P12">
         <v>4</v>
       </c>
+      <c r="P12" s="2">
+        <v>31338</v>
+      </c>
       <c r="Q12" s="3">
-        <v>31338</v>
-      </c>
-      <c r="R12" s="4">
         <v>20</v>
       </c>
-      <c r="S12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13">
+        <v>2600</v>
+      </c>
       <c r="G13">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N13">
         <v>11</v>
       </c>
       <c r="O13">
-        <v>7</v>
-      </c>
-      <c r="P13">
         <v>3</v>
       </c>
+      <c r="P13" s="2">
+        <v>43056</v>
+      </c>
       <c r="Q13" s="3">
-        <v>43056</v>
-      </c>
-      <c r="R13" s="4">
         <v>60</v>
       </c>
-      <c r="S13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
       <c r="N14">
         <v>11</v>
       </c>
       <c r="O14">
+        <v>7</v>
+      </c>
+      <c r="P14" s="2">
+        <v>37213</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>50</v>
+      </c>
+      <c r="R14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="N23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
+        <v>42886</v>
+      </c>
+      <c r="C24" s="3">
+        <v>300</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2">
+        <v>38701</v>
+      </c>
+      <c r="C25" s="3">
+        <v>400</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="2">
+        <v>36147</v>
+      </c>
+      <c r="C26" s="3">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2">
+        <v>42797</v>
+      </c>
+      <c r="C27" s="3">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>36120</v>
+      </c>
+      <c r="C28" s="3">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" t="s">
+        <v>38</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>31303</v>
+      </c>
+      <c r="C29" s="3">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="1">
+        <v>5</v>
+      </c>
+      <c r="H29" s="1">
+        <v>5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2">
+        <v>40858</v>
+      </c>
+      <c r="C30" s="3">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" s="1">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1">
+        <v>6</v>
+      </c>
+      <c r="I30" s="1">
+        <v>5</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2">
+        <v>35471</v>
+      </c>
+      <c r="C31" s="3">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="1">
+        <v>7</v>
+      </c>
+      <c r="H31" s="1">
+        <v>7</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" t="s">
+        <v>39</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="5"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <v>37516</v>
+      </c>
+      <c r="C32" s="3">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32" s="1">
+        <v>8</v>
+      </c>
+      <c r="H32" s="1">
+        <v>8</v>
+      </c>
+      <c r="I32" s="1">
+        <v>4</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" t="s">
+        <v>40</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="5"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33" s="2">
+        <v>26651</v>
+      </c>
+      <c r="C33" s="3">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="1">
+        <v>9</v>
+      </c>
+      <c r="H33" s="1">
+        <v>9</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K33" t="s">
+        <v>39</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="5"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>11</v>
       </c>
-      <c r="P14">
+      <c r="B34" s="2">
+        <v>28666</v>
+      </c>
+      <c r="C34" s="3">
+        <v>200</v>
+      </c>
+      <c r="D34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="1">
+        <v>10</v>
+      </c>
+      <c r="H34" s="1">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1">
+        <v>5</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" t="s">
+        <v>41</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="5"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="G35" s="1">
+        <v>11</v>
+      </c>
+      <c r="H35" s="1">
+        <v>11</v>
+      </c>
+      <c r="I35" s="1">
         <v>7</v>
       </c>
-      <c r="Q14" s="3">
-        <v>37213</v>
-      </c>
-      <c r="R14" s="4">
-        <v>50</v>
-      </c>
-      <c r="S14" t="s">
-        <v>53</v>
-      </c>
+      <c r="J35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" t="s">
+        <v>38</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="5"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G36" s="1">
+        <v>12</v>
+      </c>
+      <c r="H36" s="1">
+        <v>12</v>
+      </c>
+      <c r="I36" s="1">
+        <v>11</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>63</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <v>13</v>
+      </c>
+      <c r="H37" s="1">
+        <v>13</v>
+      </c>
+      <c r="I37" s="1">
+        <v>11</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>63</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1">
+        <v>14</v>
+      </c>
+      <c r="I38" s="1">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G39" s="1">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1">
+        <v>15</v>
+      </c>
+      <c r="I39" s="1">
+        <v>10</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2</v>
+      </c>
+      <c r="K39" t="s">
+        <v>67</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="N1:R1"/>
+    <mergeCell ref="G23:L23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
altered data in tables
</commit_message>
<xml_diff>
--- a/VideoGameData.xlsx
+++ b/VideoGameData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slamr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slamr\Downloads\git_fork\Project1-Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210CC5C4-5848-4D49-ABC8-C2663F98F2C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26E1BC-C79A-4AF2-89FB-4A8543EDBCF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{2D0874AA-25E2-4ECD-8491-5041E3F75BDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{2D0874AA-25E2-4ECD-8491-5041E3F75BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="84">
   <si>
     <t>ConsoleID</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Radio Shack</t>
+  </si>
+  <si>
+    <t>Smith's Marketplace</t>
   </si>
 </sst>
 </file>
@@ -319,10 +322,10 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -376,8 +379,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:R14" totalsRowShown="0">
-  <autoFilter ref="N2:R14" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:R18" totalsRowShown="0">
+  <autoFilter ref="N2:R18" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
   <tableColumns count="5">
     <tableColumn id="6" xr3:uid="{95B73333-9D34-4462-BA3A-3674305CC717}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{8F2DEC62-0DD3-4939-A7EC-C652AA40CE7C}" name="ConsoleID"/>
@@ -727,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732A0381-8E3F-4A64-ABD3-42AC0D0E900F}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,27 +753,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1093,10 +1096,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -1134,7 +1137,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11">
         <v>9</v>
@@ -1169,10 +1172,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -1207,10 +1210,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13">
-        <v>2600</v>
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
       </c>
       <c r="G13">
         <v>11</v>
@@ -1244,6 +1247,12 @@
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14">
+        <v>2600</v>
+      </c>
       <c r="G14">
         <v>12</v>
       </c>
@@ -1285,6 +1294,12 @@
       <c r="J15" t="s">
         <v>63</v>
       </c>
+      <c r="N15">
+        <v>12</v>
+      </c>
+      <c r="O15">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="G16">
@@ -1299,6 +1314,12 @@
       <c r="J16" t="s">
         <v>63</v>
       </c>
+      <c r="N16">
+        <v>13</v>
+      </c>
+      <c r="O16">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G17">
@@ -1313,15 +1334,29 @@
       <c r="J17" t="s">
         <v>67</v>
       </c>
+      <c r="N17">
+        <v>14</v>
+      </c>
+      <c r="O17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1336,18 +1371,18 @@
       <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="N23" s="4" t="s">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="N23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="4"/>
+      <c r="O23" s="5"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1409,7 +1444,7 @@
       <c r="I25" s="1">
         <v>2</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K25" t="s">
@@ -1425,7 +1460,7 @@
         <v>73</v>
       </c>
       <c r="P25" s="1"/>
-      <c r="Q25" s="5"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1449,7 +1484,7 @@
       <c r="I26" s="1">
         <v>3</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K26" t="s">
@@ -1465,7 +1500,7 @@
         <v>74</v>
       </c>
       <c r="P26" s="1"/>
-      <c r="Q26" s="5"/>
+      <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1489,7 +1524,7 @@
       <c r="I27" s="1">
         <v>4</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K27" t="s">
@@ -1505,7 +1540,7 @@
         <v>71</v>
       </c>
       <c r="P27" s="1"/>
-      <c r="Q27" s="5"/>
+      <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1529,7 +1564,7 @@
       <c r="I28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K28" t="s">
@@ -1545,7 +1580,7 @@
         <v>76</v>
       </c>
       <c r="P28" s="1"/>
-      <c r="Q28" s="5"/>
+      <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1569,7 +1604,7 @@
       <c r="I29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K29" t="s">
@@ -1585,7 +1620,7 @@
         <v>70</v>
       </c>
       <c r="P29" s="1"/>
-      <c r="Q29" s="5"/>
+      <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1609,7 +1644,7 @@
       <c r="I30" s="1">
         <v>5</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="K30" t="s">
@@ -1625,20 +1660,20 @@
         <v>78</v>
       </c>
       <c r="P30" s="1"/>
-      <c r="Q30" s="5"/>
+      <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
       <c r="B31" s="2">
-        <v>35471</v>
+        <v>42417</v>
       </c>
       <c r="C31" s="3">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G31" s="1">
         <v>7</v>
@@ -1649,7 +1684,7 @@
       <c r="I31" s="1">
         <v>3</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K31" t="s">
@@ -1661,20 +1696,20 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
-      <c r="S31" s="5"/>
+      <c r="S31" s="4"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>37516</v>
+        <v>35471</v>
       </c>
       <c r="C32" s="3">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G32" s="1">
         <v>8</v>
@@ -1685,7 +1720,7 @@
       <c r="I32" s="1">
         <v>4</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K32" t="s">
@@ -1697,20 +1732,20 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="5"/>
+      <c r="S32" s="4"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10</v>
       </c>
       <c r="B33" s="2">
-        <v>26651</v>
+        <v>37516</v>
       </c>
       <c r="C33" s="3">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G33" s="1">
         <v>9</v>
@@ -1719,7 +1754,7 @@
         <v>9</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K33" t="s">
@@ -1731,20 +1766,20 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="5"/>
+      <c r="S33" s="4"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11</v>
       </c>
       <c r="B34" s="2">
-        <v>28666</v>
+        <v>26651</v>
       </c>
       <c r="C34" s="3">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="G34" s="1">
         <v>10</v>
@@ -1755,7 +1790,7 @@
       <c r="I34" s="1">
         <v>5</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="4" t="s">
         <v>33</v>
       </c>
       <c r="K34" t="s">
@@ -1767,11 +1802,21 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" s="5"/>
+      <c r="S34" s="4"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2">
+        <v>28666</v>
+      </c>
+      <c r="C35" s="3">
+        <v>200</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
       <c r="G35" s="1">
         <v>11</v>
       </c>
@@ -1781,7 +1826,7 @@
       <c r="I35" s="1">
         <v>7</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="4" t="s">
         <v>32</v>
       </c>
       <c r="K35" t="s">
@@ -1793,7 +1838,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="5"/>
+      <c r="S35" s="4"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G36" s="1">

</xml_diff>

<commit_message>
Added seed data to the create tables file and updated the excel file with new games
</commit_message>
<xml_diff>
--- a/VideoGameData.xlsx
+++ b/VideoGameData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slamr\Downloads\git_fork\Project1-Group2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26E1BC-C79A-4AF2-89FB-4A8543EDBCF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FA8258-DC3C-4FC2-B575-D466D91B65BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{2D0874AA-25E2-4ECD-8491-5041E3F75BDD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>ConsoleID</t>
   </si>
@@ -277,6 +277,33 @@
   </si>
   <si>
     <t>Smith's Marketplace</t>
+  </si>
+  <si>
+    <t>Fallout 4</t>
+  </si>
+  <si>
+    <t>Resident Evil 6</t>
+  </si>
+  <si>
+    <t>Survival Horror</t>
+  </si>
+  <si>
+    <t>Shadow Warrior 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow Warrior </t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Action Role-playing, First-Person Shooter</t>
+  </si>
+  <si>
+    <t>Walmart</t>
+  </si>
+  <si>
+    <t>BestBuy</t>
   </si>
 </sst>
 </file>
@@ -315,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +350,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -366,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3933C6F8-BA7F-478C-9D02-D889D2DB34E8}" name="Table3" displayName="Table3" ref="G2:J19" totalsRowShown="0">
-  <autoFilter ref="G2:J19" xr:uid="{6044BB5E-06CD-4700-BC76-9E7739202459}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3933C6F8-BA7F-478C-9D02-D889D2DB34E8}" name="Table3" displayName="Table3" ref="G2:J22" totalsRowShown="0">
+  <autoFilter ref="G2:J22" xr:uid="{6044BB5E-06CD-4700-BC76-9E7739202459}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7B6C5D40-8482-4C8F-9BCF-E5A4BCCFC340}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{31940DA7-9FC6-497F-AE61-DF6930CD8FA1}" name="GameTitle"/>
@@ -379,8 +409,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:R18" totalsRowShown="0">
-  <autoFilter ref="N2:R18" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F2C6D260-4528-4784-A9DE-2A8303BF33F3}" name="Table4" displayName="Table4" ref="N2:R23" totalsRowShown="0">
+  <autoFilter ref="N2:R23" xr:uid="{0589EA6C-1C70-4EA8-A90D-907A5C75A6E4}"/>
   <tableColumns count="5">
     <tableColumn id="6" xr3:uid="{95B73333-9D34-4462-BA3A-3674305CC717}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{8F2DEC62-0DD3-4939-A7EC-C652AA40CE7C}" name="ConsoleID"/>
@@ -393,8 +423,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD363EAC-79ED-4282-BD50-7AECCC8A3080}" name="Table32" displayName="Table32" ref="G24:L42" totalsRowShown="0">
-  <autoFilter ref="G24:L42" xr:uid="{4FBBA3C7-79B4-49CF-ADF9-9C6A8B34225D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FD363EAC-79ED-4282-BD50-7AECCC8A3080}" name="Table32" displayName="Table32" ref="G24:L45" totalsRowShown="0">
+  <autoFilter ref="G24:L45" xr:uid="{4FBBA3C7-79B4-49CF-ADF9-9C6A8B34225D}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E9010659-292A-491D-A304-998FDA0DFCB9}" name="GameID"/>
     <tableColumn id="2" xr3:uid="{6B0C8F03-63B7-472D-9B7F-164D8C9739E3}" name="GameRefID"/>
@@ -408,17 +438,6 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5BAE8704-410B-4CAD-B58D-62840EB58D3E}" name="Table326" displayName="Table326" ref="N24:O30" totalsRowShown="0">
-  <autoFilter ref="N24:O30" xr:uid="{E984971F-04B5-411A-B867-E2CA8F0E8375}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{160200E6-5C9A-473B-9635-E9DD681565D6}" name="Rating"/>
-    <tableColumn id="2" xr3:uid="{E21DF097-6EF2-428B-B987-AE9AAF338A46}" name="Description"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D095B64D-2FEB-43CD-A495-6839B1A27E11}" name="Table47" displayName="Table47" ref="A23:D36" totalsRowShown="0">
   <autoFilter ref="A23:D36" xr:uid="{4788E827-78B0-45DE-AAD1-156376861332}"/>
   <tableColumns count="4">
@@ -426,6 +445,17 @@
     <tableColumn id="2" xr3:uid="{A3E5494F-2CEB-4C8D-A205-95E6C2666284}" name="PurchaseDate" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{07825330-3684-4A8C-8F99-B7BE0C4BF5EB}" name="PurchasePrice" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{CDD07CE3-7841-492D-92A3-A490D71697D6}" name="PurchaseStore"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DB55456A-94C8-4E51-9060-3A9D877C636F}" name="Table3268" displayName="Table3268" ref="N39:O45" totalsRowShown="0">
+  <autoFilter ref="N39:O45" xr:uid="{574C303A-51F8-45C7-BF3F-0B8F912EEE18}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1CF5B75E-E3F6-4B8D-A35C-30CAD9213713}" name="Rating"/>
+    <tableColumn id="2" xr3:uid="{AEE6E928-508C-4BCE-AD4D-57A4463D0268}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -728,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732A0381-8E3F-4A64-ABD3-42AC0D0E900F}">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,27 +783,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1342,6 +1372,18 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" t="s">
+        <v>39</v>
+      </c>
       <c r="N18">
         <v>15</v>
       </c>
@@ -1349,14 +1391,128 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>86</v>
+      </c>
+      <c r="N19" s="5">
+        <v>16</v>
+      </c>
+      <c r="O19">
+        <v>8</v>
+      </c>
+      <c r="P19" s="2">
+        <v>42318</v>
+      </c>
+      <c r="Q19">
+        <v>60</v>
+      </c>
+      <c r="R19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="5">
+        <v>17</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="P20" s="2">
+        <v>41197</v>
+      </c>
+      <c r="Q20">
+        <v>60</v>
+      </c>
+      <c r="R20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="5">
+        <v>18</v>
+      </c>
+      <c r="O21">
+        <v>8</v>
+      </c>
+      <c r="P21" s="2">
+        <v>42941</v>
+      </c>
+      <c r="Q21">
+        <v>50</v>
+      </c>
+      <c r="R21" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
+      <c r="N22" s="5">
+        <v>19</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22" s="2">
+        <v>41988</v>
+      </c>
+      <c r="Q22">
+        <v>45</v>
+      </c>
+      <c r="R22" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1371,18 +1527,29 @@
       <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="N23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" s="5"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="N23" s="5">
+        <v>20</v>
+      </c>
+      <c r="O23">
+        <v>8</v>
+      </c>
+      <c r="P23" s="2">
+        <v>42006</v>
+      </c>
+      <c r="Q23">
+        <v>55</v>
+      </c>
+      <c r="R23" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -1415,12 +1582,6 @@
       <c r="L24" t="s">
         <v>61</v>
       </c>
-      <c r="N24" t="s">
-        <v>6</v>
-      </c>
-      <c r="O24" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1453,14 +1614,8 @@
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="4"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -1493,14 +1648,8 @@
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="N26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="4"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="4"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -1533,14 +1682,8 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="4"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="4"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -1573,14 +1716,8 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="4"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="4"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -1613,14 +1750,8 @@
       <c r="L29">
         <v>0</v>
       </c>
-      <c r="N29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="4"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -1653,14 +1784,8 @@
       <c r="L30">
         <v>0</v>
       </c>
-      <c r="N30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="4"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1907,6 +2032,10 @@
       <c r="L38">
         <v>0</v>
       </c>
+      <c r="N38" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O38" s="6"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
@@ -1931,16 +2060,164 @@
       <c r="L39">
         <v>0</v>
       </c>
+      <c r="N39" t="s">
+        <v>6</v>
+      </c>
+      <c r="O39" t="s">
+        <v>69</v>
+      </c>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G40" s="5">
+        <v>16</v>
+      </c>
+      <c r="H40" s="5">
+        <v>16</v>
+      </c>
+      <c r="I40" s="5">
+        <v>8</v>
+      </c>
+      <c r="J40" s="5">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O40" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G41" s="5">
+        <v>17</v>
+      </c>
+      <c r="H41" s="5">
+        <v>17</v>
+      </c>
+      <c r="I41" s="5">
+        <v>8</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K41" t="s">
+        <v>86</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G42" s="5">
+        <v>18</v>
+      </c>
+      <c r="H42" s="5">
+        <v>18</v>
+      </c>
+      <c r="I42" s="5">
+        <v>8</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" t="s">
+        <v>34</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G43" s="5">
+        <v>19</v>
+      </c>
+      <c r="H43" s="5">
+        <v>19</v>
+      </c>
+      <c r="I43" s="5">
+        <v>8</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K43" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G44" s="5">
+        <v>20</v>
+      </c>
+      <c r="H44" s="5">
+        <v>20</v>
+      </c>
+      <c r="I44" s="5">
+        <v>8</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" t="s">
+        <v>90</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="N45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O45" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="N38:O38"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="G23:L23"/>
-    <mergeCell ref="N23:O23"/>
     <mergeCell ref="A22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>